<commit_message>
converted to using reaction classes
</commit_message>
<xml_diff>
--- a/example/experimental_data.xlsx
+++ b/example/experimental_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Will/Dropbox (Personal)/Python_Projects/modelling_paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Will/Dropbox (Personal)/Python_Projects/Kinetics/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="esterase_only" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>